<commit_message>
[ll] starting respin of board
</commit_message>
<xml_diff>
--- a/data/testing/board_only.xlsx
+++ b/data/testing/board_only.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6585" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6585" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Other Notes" sheetId="2" r:id="rId1"/>
     <sheet name="Issue Tracking" sheetId="1" r:id="rId2"/>
+    <sheet name="Component Status" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="77">
   <si>
     <t>Board Number</t>
   </si>
@@ -40,6 +41,222 @@
   </si>
   <si>
     <t>Fixed. Added more solder.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Board </t>
+  </si>
+  <si>
+    <t>Visual Inspection OK</t>
+  </si>
+  <si>
+    <t>Part Designator</t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>C46</t>
+  </si>
+  <si>
+    <t>C48</t>
+  </si>
+  <si>
+    <t>C49</t>
+  </si>
+  <si>
+    <t>C50</t>
+  </si>
+  <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>C27</t>
+  </si>
+  <si>
+    <t>C28</t>
+  </si>
+  <si>
+    <t>Chip</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>TAC</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>RRAMP</t>
+  </si>
+  <si>
+    <t>CRAMP</t>
+  </si>
+  <si>
+    <t>RRAMP1</t>
+  </si>
+  <si>
+    <t>CRAMP1</t>
+  </si>
+  <si>
+    <t>Active/Passive</t>
+  </si>
+  <si>
+    <t>Passive</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>Electrical Testing OK</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>D15</t>
+  </si>
+  <si>
+    <t>D17</t>
+  </si>
+  <si>
+    <t>D19</t>
+  </si>
+  <si>
+    <t>D21</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>IC2</t>
+  </si>
+  <si>
+    <t>IC3</t>
+  </si>
+  <si>
+    <t>IC4</t>
+  </si>
+  <si>
+    <t>IC5</t>
+  </si>
+  <si>
+    <t>IC6</t>
+  </si>
+  <si>
+    <t>IC8</t>
+  </si>
+  <si>
+    <t>IC9</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>IC7</t>
+  </si>
+  <si>
+    <t>IC10</t>
   </si>
 </sst>
 </file>
@@ -393,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -428,4 +645,727 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="13.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.06640625" customWidth="1"/>
+    <col min="5" max="5" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B40" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B43" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B44" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B45" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" t="s">
+        <v>39</v>
+      </c>
+      <c r="D45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B47" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" t="s">
+        <v>41</v>
+      </c>
+      <c r="D47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B48" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B49" t="s">
+        <v>35</v>
+      </c>
+      <c r="C49" t="s">
+        <v>43</v>
+      </c>
+      <c r="D49" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B50" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" t="s">
+        <v>44</v>
+      </c>
+      <c r="D50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B51" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" t="s">
+        <v>45</v>
+      </c>
+      <c r="D51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B52" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" t="s">
+        <v>46</v>
+      </c>
+      <c r="D52" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B53" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" t="s">
+        <v>47</v>
+      </c>
+      <c r="D53" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B54" t="s">
+        <v>35</v>
+      </c>
+      <c r="C54" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B55" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55" t="s">
+        <v>51</v>
+      </c>
+      <c r="D55" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B56" t="s">
+        <v>35</v>
+      </c>
+      <c r="C56" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B57" t="s">
+        <v>35</v>
+      </c>
+      <c r="C57" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B58" t="s">
+        <v>35</v>
+      </c>
+      <c r="C58" t="s">
+        <v>75</v>
+      </c>
+      <c r="D58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B59" t="s">
+        <v>35</v>
+      </c>
+      <c r="C59" t="s">
+        <v>71</v>
+      </c>
+      <c r="D59" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B60" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" t="s">
+        <v>72</v>
+      </c>
+      <c r="D60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B61" t="s">
+        <v>35</v>
+      </c>
+      <c r="C61" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B62" t="s">
+        <v>35</v>
+      </c>
+      <c r="C62" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B63" t="s">
+        <v>35</v>
+      </c>
+      <c r="C63" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>